<commit_message>
Updated Muchow Experiment and graphed out extinction graph
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/MuchowObserved.xlsx
+++ b/Prototypes/Mungbean/MuchowObserved.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A43826-CF5E-4C25-B1D2-4F339C64EB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897556B-7C4F-4A1A-9494-D944D637BF2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
   </bookViews>
   <sheets>
-    <sheet name="observed" sheetId="1" r:id="rId1"/>
+    <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
   <si>
     <t>Location</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Gatton</t>
   </si>
   <si>
-    <t>GattonSowJan9</t>
-  </si>
-  <si>
     <t>Katherine1989SowJan10</t>
   </si>
   <si>
@@ -89,18 +86,12 @@
     <t>KatherineJan28WaterRainfed</t>
   </si>
   <si>
-    <t>Katherine1988</t>
-  </si>
-  <si>
     <t>Soybean.Grain.N</t>
   </si>
   <si>
     <t>Soybean.Grain.NHI</t>
   </si>
   <si>
-    <t>Soybean..AboveGround.N</t>
-  </si>
-  <si>
     <t>Soybean..Pod.N</t>
   </si>
   <si>
@@ -111,6 +102,15 @@
   </si>
   <si>
     <t>Katherine</t>
+  </si>
+  <si>
+    <t>Soybean.AboveGround.N</t>
+  </si>
+  <si>
+    <t>GattonJan91990</t>
+  </si>
+  <si>
+    <t>RadiationIntercepted</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +192,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,11 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE48974-63BC-46EF-A3A1-52070277FA63}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -522,9 +525,12 @@
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="15" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34.5">
+    <row r="1" spans="1:19" ht="34.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
@@ -550,19 +556,19 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>8</v>
@@ -573,13 +579,16 @@
       <c r="P1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6">
         <v>32911</v>
@@ -593,13 +602,14 @@
       <c r="I2">
         <v>4.53</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6">
         <v>32918</v>
@@ -607,13 +617,18 @@
       <c r="I3">
         <v>7.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3">
+        <v>0.35</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6">
         <v>32919</v>
@@ -624,13 +639,15 @@
       <c r="F4">
         <v>1.77</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6">
         <v>32926</v>
@@ -644,13 +661,15 @@
       <c r="I5">
         <v>11.32</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6">
         <v>32932</v>
@@ -658,13 +677,15 @@
       <c r="I6">
         <v>13.82</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6">
         <v>32933</v>
@@ -675,13 +696,16 @@
       <c r="F7">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6">
         <v>32939</v>
@@ -692,13 +716,16 @@
       <c r="O8">
         <v>85.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C9" s="6">
         <v>32940</v>
@@ -712,13 +739,16 @@
       <c r="I9">
         <v>16.37</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <v>32946</v>
@@ -732,13 +762,16 @@
       <c r="O10">
         <v>209.13</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6">
         <v>32947</v>
@@ -749,13 +782,16 @@
       <c r="F11">
         <v>1.31</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6">
         <v>32962</v>
@@ -763,13 +799,16 @@
       <c r="O12">
         <v>368.79</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C13" s="6">
         <v>32963</v>
@@ -786,30 +825,39 @@
       <c r="L13">
         <v>4.3499999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O14">
         <v>10.27</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="C15" s="6">
+        <v>32962</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>0.31</v>
@@ -836,198 +884,235 @@
         <v>10.6</v>
       </c>
       <c r="P15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <v>32588</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H16">
+        <v>226</v>
+      </c>
+      <c r="I16">
+        <v>5.53</v>
+      </c>
+      <c r="K16">
+        <v>6.54</v>
+      </c>
+      <c r="M16">
+        <v>0.34</v>
+      </c>
+      <c r="N16">
+        <v>155</v>
+      </c>
+      <c r="O16">
+        <v>5.34</v>
+      </c>
+      <c r="P16">
+        <v>42</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6">
+        <v>32560</v>
+      </c>
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
       <c r="G17">
-        <v>0.28000000000000003</v>
+        <v>0.17</v>
       </c>
       <c r="H17">
-        <v>226</v>
+        <v>273</v>
       </c>
       <c r="I17">
-        <v>5.53</v>
+        <v>5.8</v>
       </c>
       <c r="K17">
-        <v>6.54</v>
+        <v>2.78</v>
       </c>
       <c r="M17">
-        <v>0.34</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="N17">
-        <v>155</v>
+        <v>60.8</v>
       </c>
       <c r="O17">
-        <v>5.34</v>
+        <v>12.1</v>
       </c>
       <c r="P17">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="G18">
-        <v>0.17</v>
-      </c>
-      <c r="H18">
-        <v>273</v>
-      </c>
-      <c r="I18">
-        <v>5.8</v>
-      </c>
-      <c r="K18">
-        <v>2.78</v>
-      </c>
-      <c r="M18">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="N18">
-        <v>60.8</v>
-      </c>
-      <c r="O18">
-        <v>12.1</v>
-      </c>
-      <c r="P18">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="C18" s="6">
+        <v>32585</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6">
-        <v>32585</v>
+        <v>32592</v>
       </c>
       <c r="L19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>4.55</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6">
-        <v>32592</v>
+        <v>32600</v>
       </c>
       <c r="L20">
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>4.74</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="6">
-        <v>32600</v>
+        <v>32628</v>
       </c>
       <c r="L21">
-        <v>4.74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="6">
-        <v>32628</v>
-      </c>
-      <c r="L22">
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>32558</v>
+      </c>
+      <c r="I22">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="6">
-        <v>36210</v>
+        <v>32564</v>
       </c>
       <c r="I23">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>1.78</v>
+      </c>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6">
-        <v>36216</v>
-      </c>
+        <v>32570</v>
+      </c>
+      <c r="D24" s="7"/>
       <c r="I24">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
+        <v>3.88</v>
+      </c>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="6">
-        <v>36222</v>
+        <v>32571</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="I25">
-        <v>3.88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="6">
-        <v>36231</v>
+        <v>32579</v>
       </c>
       <c r="I26">
         <v>7.17</v>
@@ -1035,16 +1120,19 @@
       <c r="O26">
         <v>10.234</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="6">
-        <v>36237</v>
+        <v>32585</v>
       </c>
       <c r="I27">
         <v>10.16</v>
@@ -1052,16 +1140,19 @@
       <c r="O27">
         <v>68.947999999999993</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="6">
-        <v>36245</v>
+        <v>32593</v>
       </c>
       <c r="I28">
         <v>10.76</v>
@@ -1069,30 +1160,39 @@
       <c r="O28">
         <v>165.87700000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6">
-        <v>36253</v>
+        <v>32601</v>
       </c>
       <c r="O29">
         <v>191.48599999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C30" s="6">
+        <v>32578</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <v>0.25</v>
@@ -1121,13 +1221,16 @@
       <c r="P30">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="6">
         <v>32585</v>
@@ -1135,13 +1238,16 @@
       <c r="L31">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="6">
         <v>32592</v>
@@ -1149,13 +1255,16 @@
       <c r="L32">
         <v>4.28</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="6">
         <v>32595</v>
@@ -1163,13 +1272,16 @@
       <c r="L33">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="6">
         <v>32628</v>
@@ -1177,173 +1289,212 @@
       <c r="L34">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="6">
-        <v>36209</v>
+        <v>32557</v>
       </c>
       <c r="I35">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="6">
-        <v>36215</v>
+        <v>32563</v>
       </c>
       <c r="I36">
         <v>2.41</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="6">
-        <v>36221</v>
+        <v>32569</v>
       </c>
       <c r="I37">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="6">
-        <v>36229</v>
+        <v>32577</v>
       </c>
       <c r="I38">
         <v>4.33</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="6">
-        <v>36230</v>
+        <v>32578</v>
       </c>
       <c r="D39" s="7"/>
       <c r="O39">
         <v>3.6360000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="6">
-        <v>36236</v>
+        <v>32584</v>
       </c>
       <c r="I40">
         <v>4.91</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6">
-        <v>36237</v>
+        <v>32585</v>
       </c>
       <c r="D41" s="7"/>
       <c r="O41">
         <v>60.91</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" s="6">
-        <v>36244</v>
+        <v>32592</v>
       </c>
       <c r="I42">
         <v>6.69</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="6">
-        <v>36247</v>
+        <v>32595</v>
       </c>
       <c r="O43">
         <v>125.6</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" s="6">
-        <v>36248</v>
+        <v>32596</v>
       </c>
       <c r="I44">
         <v>8.17</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="6">
-        <v>36253</v>
+        <v>32601</v>
       </c>
       <c r="D45" s="7"/>
       <c r="I45">
         <v>12.56</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C46" s="6">
+        <v>32578</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G46">
         <v>0.24</v>
@@ -1372,6 +1523,174 @@
       <c r="P46">
         <v>42</v>
       </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6"/>
+    </row>
+    <row r="49" spans="17:18">
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="17:18">
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+    </row>
+    <row r="51" spans="17:18">
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+    </row>
+    <row r="52" spans="17:18">
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="17:18">
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+    </row>
+    <row r="54" spans="17:18">
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+    </row>
+    <row r="55" spans="17:18">
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+    </row>
+    <row r="56" spans="17:18">
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+    </row>
+    <row r="57" spans="17:18">
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+    </row>
+    <row r="58" spans="17:18">
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+    </row>
+    <row r="59" spans="17:18">
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+    </row>
+    <row r="60" spans="17:18">
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+    </row>
+    <row r="61" spans="17:18">
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+    </row>
+    <row r="62" spans="17:18">
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+    </row>
+    <row r="63" spans="17:18">
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+    </row>
+    <row r="64" spans="17:18">
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+    </row>
+    <row r="65" spans="17:18">
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+    </row>
+    <row r="66" spans="17:18">
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+    </row>
+    <row r="67" spans="17:18">
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+    </row>
+    <row r="68" spans="17:18">
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+    </row>
+    <row r="69" spans="17:18">
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+    </row>
+    <row r="70" spans="17:18">
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+    </row>
+    <row r="71" spans="17:18">
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+    </row>
+    <row r="72" spans="17:18">
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+    </row>
+    <row r="73" spans="17:18">
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+    </row>
+    <row r="74" spans="17:18">
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+    </row>
+    <row r="75" spans="17:18">
+      <c r="Q75" s="6"/>
+      <c r="R75" s="6"/>
+    </row>
+    <row r="76" spans="17:18">
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+    </row>
+    <row r="77" spans="17:18">
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+    </row>
+    <row r="78" spans="17:18">
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+    </row>
+    <row r="79" spans="17:18">
+      <c r="R79" s="6"/>
+    </row>
+    <row r="80" spans="17:18">
+      <c r="R80" s="6"/>
+    </row>
+    <row r="81" spans="18:18">
+      <c r="R81" s="6"/>
+    </row>
+    <row r="82" spans="18:18">
+      <c r="R82" s="6"/>
+    </row>
+    <row r="83" spans="18:18">
+      <c r="R83" s="6"/>
+    </row>
+    <row r="84" spans="18:18">
+      <c r="R84" s="6"/>
+    </row>
+    <row r="85" spans="18:18">
+      <c r="R85" s="6"/>
+    </row>
+    <row r="86" spans="18:18">
+      <c r="R86" s="6"/>
+    </row>
+    <row r="87" spans="18:18">
+      <c r="R87" s="6"/>
+    </row>
+    <row r="88" spans="18:18">
+      <c r="R88" s="6"/>
+    </row>
+    <row r="89" spans="18:18">
+      <c r="R89" s="6"/>
+    </row>
+    <row r="90" spans="18:18">
+      <c r="R90" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P46">

</xml_diff>

<commit_message>
Adjusting the parameters to capture stem weight.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/MuchowObserved.xlsx
+++ b/Prototypes/Mungbean/MuchowObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897556B-7C4F-4A1A-9494-D944D637BF2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFB72D-7C41-49C0-819C-24C8998F42D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
   <si>
     <t>Location</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Soybean..Pod.N</t>
-  </si>
-  <si>
-    <t>29/02/1990</t>
   </si>
   <si>
     <t>Soybean.Leaf.SLN</t>
@@ -514,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
@@ -556,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -580,7 +577,7 @@
         <v>10</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -588,7 +585,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6">
         <v>32911</v>
@@ -609,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6">
         <v>32918</v>
@@ -628,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6">
         <v>32919</v>
@@ -647,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6">
         <v>32926</v>
@@ -669,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6">
         <v>32932</v>
@@ -685,7 +682,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6">
         <v>32933</v>
@@ -705,7 +702,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6">
         <v>32939</v>
@@ -725,7 +722,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6">
         <v>32940</v>
@@ -748,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
         <v>32946</v>
@@ -771,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6">
         <v>32947</v>
@@ -791,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6">
         <v>32962</v>
@@ -808,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
         <v>32963</v>
@@ -834,10 +831,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C14" s="6">
+        <v>32961</v>
       </c>
       <c r="O14">
         <v>10.27</v>
@@ -851,7 +848,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6">
         <v>32962</v>
@@ -892,7 +889,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -933,7 +930,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -974,7 +971,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -991,7 +988,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -1008,7 +1005,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -1025,7 +1022,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -1042,7 +1039,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -1059,7 +1056,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -1076,7 +1073,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
@@ -1106,7 +1103,7 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -1146,7 +1143,7 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -1166,7 +1163,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -1183,7 +1180,7 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
@@ -1227,7 +1224,7 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -1244,7 +1241,7 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -1261,7 +1258,7 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -1278,7 +1275,7 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -1295,7 +1292,7 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -1312,7 +1309,7 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
@@ -1329,7 +1326,7 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
@@ -1346,7 +1343,7 @@
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -1363,7 +1360,7 @@
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>16</v>
@@ -1381,7 +1378,7 @@
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -1398,7 +1395,7 @@
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -1416,7 +1413,7 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
@@ -1450,7 +1447,7 @@
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
@@ -1467,7 +1464,7 @@
     </row>
     <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -1485,7 +1482,7 @@
     </row>
     <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Additional Muchow study added. Calibration focused on Muchow Gatton
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/MuchowObserved.xlsx
+++ b/Prototypes/Mungbean/MuchowObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6301AF0B-A0D6-4F5E-A7BB-1B7115E26257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3CBC90-3E37-4D32-BDB1-FF436D5848F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="38">
   <si>
     <t>Location</t>
   </si>
@@ -107,9 +107,6 @@
     <t>RadiationIntercepted</t>
   </si>
   <si>
-    <t>Soybean.Phenology.GrainfillingDAS</t>
-  </si>
-  <si>
     <t>StartGrainFill</t>
   </si>
   <si>
@@ -126,13 +123,37 @@
   </si>
   <si>
     <t>Soybean.Stem.N</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Live.Nconc</t>
+  </si>
+  <si>
+    <t>Soybean.Stem.Live.Nconc</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.StartGrainfillingDAS</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Kimberly1980Dens10</t>
+  </si>
+  <si>
+    <t>Kimberly1980Dens27</t>
+  </si>
+  <si>
+    <t>Kimberly1980Dens50</t>
+  </si>
+  <si>
+    <t>StemPodWt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,28 +550,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE48974-63BC-46EF-A3A1-52070277FA63}">
-  <dimension ref="A1:W68"/>
+  <dimension ref="A1:Y141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D27:D28"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" customWidth="1"/>
-    <col min="19" max="22" width="14.5703125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" style="6" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" customWidth="1"/>
+    <col min="13" max="17" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="23" width="14.5703125" style="10" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="10" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45.75">
+    <row r="1" spans="1:25" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +603,7 @@
         <v>21</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>17</v>
@@ -597,28 +621,37 @@
         <v>9</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="T1" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="V1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="Y1" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -638,7 +671,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -651,11 +684,11 @@
       <c r="I3">
         <v>7.18</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -672,7 +705,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -692,7 +725,7 @@
         <v>11.32</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -703,7 +736,7 @@
         <v>32932</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6">
         <v>508</v>
@@ -717,21 +750,29 @@
       <c r="O6">
         <v>10.6</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="10">
+      <c r="S6" s="6"/>
+      <c r="T6" s="10">
         <v>264.16000000000003</v>
       </c>
-      <c r="T6" s="10">
+      <c r="U6" s="10">
         <v>243.83999999999997</v>
       </c>
-      <c r="U6" s="10">
+      <c r="V6" s="10">
         <v>10.488000000000001</v>
       </c>
-      <c r="V6" s="10">
+      <c r="W6" s="10">
         <v>3.3119999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="X6" s="10">
+        <f>V6/T6</f>
+        <v>3.9703210175651121E-2</v>
+      </c>
+      <c r="Y6" s="10">
+        <f>W6/U6</f>
+        <v>1.3582677165354329E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -747,9 +788,9 @@
       <c r="F7">
         <v>1.81</v>
       </c>
-      <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -765,9 +806,9 @@
       <c r="O8">
         <v>85.05</v>
       </c>
-      <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -786,9 +827,9 @@
       <c r="I9">
         <v>16.37</v>
       </c>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -807,9 +848,9 @@
       <c r="O10">
         <v>209.13</v>
       </c>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -825,9 +866,9 @@
       <c r="F11">
         <v>1.31</v>
       </c>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -873,27 +914,37 @@
       <c r="O12">
         <v>370.6</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>50</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>80</v>
       </c>
-      <c r="R12" s="6"/>
-      <c r="S12" s="10">
+      <c r="S12" s="6"/>
+      <c r="T12" s="10">
         <v>169.76000000000002</v>
       </c>
-      <c r="T12" s="10">
-        <v>190.33999999999997</v>
-      </c>
       <c r="U12" s="10">
+        <f>U6+53.5</f>
+        <v>297.33999999999997</v>
+      </c>
+      <c r="V12" s="10">
         <v>3.6180000000000012</v>
       </c>
-      <c r="V12" s="10">
-        <v>2.2319999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12" s="10">
+        <f>W6+1.08</f>
+        <v>4.3919999999999995</v>
+      </c>
+      <c r="X12" s="10">
+        <f>V12/T12</f>
+        <v>2.1312441093308203E-2</v>
+      </c>
+      <c r="Y12" s="10">
+        <f>W12/U12</f>
+        <v>1.4770969260778906E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -904,7 +955,7 @@
         <v>32588</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13">
         <v>226</v>
@@ -915,9 +966,9 @@
       <c r="O13">
         <v>5.34</v>
       </c>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -951,15 +1002,15 @@
       <c r="O14">
         <v>228.34</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>42</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>67</v>
       </c>
-      <c r="R14" s="6"/>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -970,7 +1021,7 @@
         <v>32560</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15">
         <v>273</v>
@@ -981,9 +1032,9 @@
       <c r="O15">
         <v>12.1</v>
       </c>
-      <c r="R15" s="6"/>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1017,15 +1068,15 @@
       <c r="O16">
         <v>86.399999999999991</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>42</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>63</v>
       </c>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1038,9 +1089,9 @@
       <c r="I17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R17" s="6"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1053,9 +1104,9 @@
       <c r="I18">
         <v>1.78</v>
       </c>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1069,9 +1120,9 @@
       <c r="I19">
         <v>3.88</v>
       </c>
-      <c r="R19" s="6"/>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1082,7 +1133,7 @@
         <v>32578</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20">
         <v>253</v>
@@ -1096,21 +1147,29 @@
       <c r="O20">
         <v>4.88</v>
       </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="10">
+      <c r="S20" s="6"/>
+      <c r="T20" s="10">
         <v>134.09</v>
       </c>
-      <c r="T20" s="10">
+      <c r="U20" s="10">
         <v>118.91</v>
       </c>
-      <c r="U20" s="10">
+      <c r="V20" s="10">
         <v>5.9049000000000005</v>
       </c>
-      <c r="V20" s="10">
+      <c r="W20" s="10">
         <v>1.3850999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="X20" s="10">
+        <f>V20/T20</f>
+        <v>4.4036840927735105E-2</v>
+      </c>
+      <c r="Y20" s="10">
+        <f>W20/U20</f>
+        <v>1.1648305441089897E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1123,9 +1182,9 @@
       <c r="L21">
         <v>0.05</v>
       </c>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1141,9 +1200,9 @@
       <c r="O22">
         <v>68.947999999999993</v>
       </c>
-      <c r="R22" s="6"/>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1156,9 +1215,9 @@
       <c r="L23">
         <v>4.5499999999999999E-2</v>
       </c>
-      <c r="R23" s="6"/>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1174,9 +1233,9 @@
       <c r="O24">
         <v>165.87700000000001</v>
       </c>
-      <c r="R24" s="6"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1216,27 +1275,35 @@
       <c r="O25">
         <v>191.88</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>42</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>65</v>
       </c>
-      <c r="R25" s="6"/>
-      <c r="S25" s="10">
+      <c r="S25" s="6"/>
+      <c r="T25" s="10">
         <v>141.55000000000001</v>
       </c>
-      <c r="T25" s="10">
+      <c r="U25" s="10">
         <v>196.20999999999998</v>
       </c>
-      <c r="U25" s="10">
+      <c r="V25" s="10">
         <v>4.3749000000000002</v>
       </c>
-      <c r="V25" s="10">
+      <c r="W25" s="10">
         <v>1.6850999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="X25" s="10">
+        <f>V25/T25</f>
+        <v>3.090709996467679E-2</v>
+      </c>
+      <c r="Y25" s="10">
+        <f>W25/U25</f>
+        <v>8.5882472860710456E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1249,9 +1316,9 @@
       <c r="I26">
         <v>0.78</v>
       </c>
-      <c r="R26" s="6"/>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1264,9 +1331,9 @@
       <c r="I27">
         <v>2.41</v>
       </c>
-      <c r="R27" s="6"/>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1279,9 +1346,9 @@
       <c r="I28">
         <v>4.04</v>
       </c>
-      <c r="R28" s="6"/>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1294,9 +1361,9 @@
       <c r="I29">
         <v>4.33</v>
       </c>
-      <c r="R29" s="6"/>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1307,7 +1374,7 @@
         <v>32578</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30">
         <v>180</v>
@@ -1321,21 +1388,29 @@
       <c r="O30">
         <v>4.28</v>
       </c>
-      <c r="R30" s="6"/>
-      <c r="S30" s="10">
+      <c r="S30" s="6"/>
+      <c r="T30" s="10">
         <v>84.6</v>
       </c>
-      <c r="T30" s="10">
+      <c r="U30" s="10">
         <v>95.4</v>
       </c>
-      <c r="U30" s="10">
+      <c r="V30" s="10">
         <v>3.0825000000000005</v>
       </c>
-      <c r="V30" s="10">
+      <c r="W30" s="10">
         <v>1.0274999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="X30" s="10">
+        <f>V30/T30</f>
+        <v>3.6436170212765968E-2</v>
+      </c>
+      <c r="Y30" s="10">
+        <f>W30/U30</f>
+        <v>1.0770440251572325E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1348,9 +1423,9 @@
       <c r="I31">
         <v>4.91</v>
       </c>
-      <c r="R31" s="6"/>
-    </row>
-    <row r="32" spans="1:22">
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1366,9 +1441,9 @@
       <c r="O32">
         <v>60.91</v>
       </c>
-      <c r="R32" s="6"/>
-    </row>
-    <row r="33" spans="1:22">
+      <c r="S32" s="6"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1384,9 +1459,9 @@
       <c r="L33">
         <v>4.2800000000000005E-2</v>
       </c>
-      <c r="R33" s="6"/>
-    </row>
-    <row r="34" spans="1:22">
+      <c r="S33" s="6"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1399,9 +1474,9 @@
       <c r="L34">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="R34" s="6"/>
-    </row>
-    <row r="35" spans="1:22">
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1438,27 +1513,35 @@
       <c r="O35">
         <v>125.28</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>42</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>60</v>
       </c>
-      <c r="R35" s="6"/>
-      <c r="S35" s="10">
+      <c r="S35" s="6"/>
+      <c r="T35" s="10">
         <v>91.47</v>
       </c>
-      <c r="T35" s="10">
+      <c r="U35" s="10">
         <v>137.4</v>
       </c>
-      <c r="U35" s="10">
+      <c r="V35" s="10">
         <v>3.0425000000000004</v>
       </c>
-      <c r="V35" s="10">
+      <c r="W35" s="10">
         <v>1.2074999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:22">
+      <c r="X35" s="10">
+        <f>V35/T35</f>
+        <v>3.3262271783098291E-2</v>
+      </c>
+      <c r="Y35" s="10">
+        <f>W35/U35</f>
+        <v>8.7882096069868982E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1472,106 +1555,1163 @@
       <c r="I36">
         <v>12.56</v>
       </c>
-      <c r="R36" s="6"/>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="R37" s="6"/>
-    </row>
-    <row r="38" spans="1:22">
-      <c r="R38" s="6"/>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="R39" s="6"/>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="R40" s="6"/>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="R41" s="6"/>
-    </row>
-    <row r="42" spans="1:22">
-      <c r="R42" s="6"/>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="R43" s="6"/>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="R44" s="6"/>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="R45" s="6"/>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="R46" s="6"/>
-    </row>
-    <row r="47" spans="1:22">
-      <c r="R47" s="6"/>
-    </row>
-    <row r="48" spans="1:22">
-      <c r="R48" s="6"/>
-    </row>
-    <row r="49" spans="18:18">
-      <c r="R49" s="6"/>
-    </row>
-    <row r="50" spans="18:18">
-      <c r="R50" s="6"/>
-    </row>
-    <row r="51" spans="18:18">
-      <c r="R51" s="6"/>
-    </row>
-    <row r="52" spans="18:18">
-      <c r="R52" s="6"/>
-    </row>
-    <row r="53" spans="18:18">
-      <c r="R53" s="6"/>
-    </row>
-    <row r="54" spans="18:18">
-      <c r="R54" s="6"/>
-    </row>
-    <row r="55" spans="18:18">
-      <c r="R55" s="6"/>
-    </row>
-    <row r="56" spans="18:18">
-      <c r="R56" s="6"/>
-    </row>
-    <row r="57" spans="18:18">
-      <c r="R57" s="6"/>
-    </row>
-    <row r="58" spans="18:18">
-      <c r="R58" s="6"/>
-    </row>
-    <row r="59" spans="18:18">
-      <c r="R59" s="6"/>
-    </row>
-    <row r="60" spans="18:18">
-      <c r="R60" s="6"/>
-    </row>
-    <row r="61" spans="18:18">
-      <c r="R61" s="6"/>
-    </row>
-    <row r="62" spans="18:18">
-      <c r="R62" s="6"/>
-    </row>
-    <row r="63" spans="18:18">
-      <c r="R63" s="6"/>
-    </row>
-    <row r="64" spans="18:18">
-      <c r="R64" s="6"/>
-    </row>
-    <row r="65" spans="18:18">
-      <c r="R65" s="6"/>
-    </row>
-    <row r="66" spans="18:18">
-      <c r="R66" s="6"/>
-    </row>
-    <row r="67" spans="18:18">
-      <c r="R67" s="6"/>
-    </row>
-    <row r="68" spans="18:18">
-      <c r="R68" s="6"/>
+      <c r="S36" s="6"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="6">
+        <v>29262</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="S37">
+        <v>66.064981949458399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="6">
+        <v>29270</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="S38">
+        <v>91.046931407942196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="6">
+        <v>29279</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="S39">
+        <v>81.083032490974702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="6">
+        <v>29290</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="S40">
+        <v>77.617328519855604</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="6">
+        <v>29299</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="S41">
+        <v>70.974729241877199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="6">
+        <v>29262</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="S42">
+        <v>84.038004750593899</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="6">
+        <v>29270</v>
+      </c>
+      <c r="I43" s="6"/>
+      <c r="S43">
+        <v>96.152019002375397</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="6">
+        <v>29279</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="S44">
+        <v>88.171021377672304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="6">
+        <v>29290</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="S45">
+        <v>79.762470308788707</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="6">
+        <v>29299</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="S46">
+        <v>80.190023752969196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="6">
+        <v>29262</v>
+      </c>
+      <c r="I47" s="6"/>
+      <c r="S47">
+        <v>95.107913669064899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="6">
+        <v>29270</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="S48">
+        <v>98.561151079136806</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="6">
+        <v>29279</v>
+      </c>
+      <c r="I49" s="6"/>
+      <c r="S49">
+        <v>97.410071942446095</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="6">
+        <v>29290</v>
+      </c>
+      <c r="I50" s="6"/>
+      <c r="S50">
+        <v>91.654676258992893</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="6">
+        <v>29299</v>
+      </c>
+      <c r="I51" s="6"/>
+      <c r="S51">
+        <v>91.366906474820297</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="6">
+        <v>29248</v>
+      </c>
+      <c r="H52">
+        <v>0.32111198190552498</v>
+      </c>
+      <c r="I52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="S52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="6">
+        <v>29255</v>
+      </c>
+      <c r="H53">
+        <v>1.09776133645736</v>
+      </c>
+      <c r="I53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="6">
+        <v>29262</v>
+      </c>
+      <c r="H54">
+        <v>1.7268245737280801</v>
+      </c>
+      <c r="I54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="S54" s="6"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="6">
+        <v>29268</v>
+      </c>
+      <c r="H55">
+        <v>2.7213304475296698</v>
+      </c>
+      <c r="I55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="S55" s="6"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="6">
+        <v>29276</v>
+      </c>
+      <c r="H56">
+        <v>4.1666551613518799</v>
+      </c>
+      <c r="I56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="S56" s="6"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="6">
+        <v>29283</v>
+      </c>
+      <c r="H57">
+        <v>4.9589382083382398</v>
+      </c>
+      <c r="I57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="S57" s="6"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="6">
+        <v>29290</v>
+      </c>
+      <c r="H58">
+        <v>4.9658210937087599</v>
+      </c>
+      <c r="I58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="S58" s="6"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="6">
+        <v>29296</v>
+      </c>
+      <c r="H59">
+        <v>6.2712953224804302</v>
+      </c>
+      <c r="I59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="O59">
+        <v>19.285714285714199</v>
+      </c>
+      <c r="Q59">
+        <v>5.4533789563713199E-3</v>
+      </c>
+      <c r="S59" s="6"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="6">
+        <v>29301</v>
+      </c>
+      <c r="H60">
+        <v>6.0141515371777299</v>
+      </c>
+      <c r="I60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="O60">
+        <v>26.071428571428601</v>
+      </c>
+      <c r="Q60">
+        <v>0.125106928999143</v>
+      </c>
+      <c r="S60" s="6"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="6">
+        <v>29248</v>
+      </c>
+      <c r="H61">
+        <v>0.16554659043380501</v>
+      </c>
+      <c r="I61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="O61">
+        <v>31.964285714285701</v>
+      </c>
+      <c r="Q61">
+        <v>0.51502352437981003</v>
+      </c>
+      <c r="S61" s="6"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="6">
+        <v>29255</v>
+      </c>
+      <c r="H62">
+        <v>0.48347904476108899</v>
+      </c>
+      <c r="I62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="O62">
+        <v>39.107142857142797</v>
+      </c>
+      <c r="Q62">
+        <v>0.97567365269460904</v>
+      </c>
+      <c r="S62" s="6"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="6">
+        <v>29262</v>
+      </c>
+      <c r="H63">
+        <v>1.1902640672776601</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="O63">
+        <v>46.25</v>
+      </c>
+      <c r="Q63">
+        <v>1.5081800684345501</v>
+      </c>
+      <c r="S63" s="6"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="6">
+        <v>29268</v>
+      </c>
+      <c r="H64">
+        <v>2.27820663274629</v>
+      </c>
+      <c r="I64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="O64">
+        <v>53.035714285714299</v>
+      </c>
+      <c r="Q64">
+        <v>1.3044803250641499</v>
+      </c>
+      <c r="S64" s="6"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="6">
+        <v>29276</v>
+      </c>
+      <c r="H65">
+        <v>3.7157348038479201</v>
+      </c>
+      <c r="I65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="O65">
+        <v>60.892857142857103</v>
+      </c>
+      <c r="Q65">
+        <v>1.0279619332762999</v>
+      </c>
+      <c r="S65" s="6"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="6">
+        <v>29283</v>
+      </c>
+      <c r="H66">
+        <v>4.1968667643941604</v>
+      </c>
+      <c r="I66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="O66">
+        <v>67.142857142857196</v>
+      </c>
+      <c r="Q66">
+        <v>1.09420444824636</v>
+      </c>
+      <c r="S66" s="6"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="6">
+        <v>29290</v>
+      </c>
+      <c r="H67">
+        <v>5.0824240750742096</v>
+      </c>
+      <c r="I67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="O67">
+        <v>71.785714285714306</v>
+      </c>
+      <c r="Q67">
+        <v>0.98224978614199898</v>
+      </c>
+      <c r="S67" s="6"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="6">
+        <v>29296</v>
+      </c>
+      <c r="H68">
+        <v>5.29152978725996</v>
+      </c>
+      <c r="I68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="O68">
+        <v>19.285714285714199</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="S68" s="6"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="6">
+        <v>29301</v>
+      </c>
+      <c r="H69">
+        <v>5.4775910307273099</v>
+      </c>
+      <c r="I69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="O69">
+        <v>26.071428571428601</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="6">
+        <v>29248</v>
+      </c>
+      <c r="H70">
+        <v>8.7743591201277796E-2</v>
+      </c>
+      <c r="I70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="O70">
+        <v>32.5</v>
+      </c>
+      <c r="Q70">
+        <v>0.137296834901624</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="6">
+        <v>29255</v>
+      </c>
+      <c r="H71">
+        <v>0.226863150371757</v>
+      </c>
+      <c r="I71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="O71">
+        <v>39.107142857142797</v>
+      </c>
+      <c r="Q71">
+        <v>0.68824850299400997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="6">
+        <v>29262</v>
+      </c>
+      <c r="H72">
+        <v>0.73926249578702496</v>
+      </c>
+      <c r="I72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="O72">
+        <v>46.071428571428598</v>
+      </c>
+      <c r="Q72">
+        <v>1.7418733960650099</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="6">
+        <v>29268</v>
+      </c>
+      <c r="H73">
+        <v>1.3528341650999101</v>
+      </c>
+      <c r="I73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="O73">
+        <v>53.214285714285701</v>
+      </c>
+      <c r="Q73">
+        <v>2.3821642429426801</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" s="6">
+        <v>29276</v>
+      </c>
+      <c r="H74">
+        <v>2.6347969447298198</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="O74">
+        <v>59.821428571428498</v>
+      </c>
+      <c r="Q74">
+        <v>3.49000213857998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="6">
+        <v>29283</v>
+      </c>
+      <c r="H75">
+        <v>3.7147399325111699</v>
+      </c>
+      <c r="I75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="O75">
+        <v>67.142857142857196</v>
+      </c>
+      <c r="Q75">
+        <v>3.6630667236954602</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="6">
+        <v>29290</v>
+      </c>
+      <c r="H76">
+        <v>4.1103738685876401</v>
+      </c>
+      <c r="I76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="O76">
+        <v>71.428571428571402</v>
+      </c>
+      <c r="Q76">
+        <v>3.9286783575705702</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="6">
+        <v>29296</v>
+      </c>
+      <c r="H77">
+        <v>5.1981743095795903</v>
+      </c>
+      <c r="I77" s="6"/>
+      <c r="K77" s="6"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="6">
+        <v>29301</v>
+      </c>
+      <c r="H78">
+        <v>5.3687033780957698</v>
+      </c>
+      <c r="I78" s="6"/>
+      <c r="K78" s="6"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B79" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="6">
+        <v>29249</v>
+      </c>
+      <c r="I79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="T79">
+        <v>0.54533789563713198</v>
+      </c>
+      <c r="U79"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="6">
+        <v>29256</v>
+      </c>
+      <c r="I80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <v>12.5106928999143</v>
+      </c>
+      <c r="U80"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="6">
+        <v>29262</v>
+      </c>
+      <c r="I81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="P81">
+        <v>13.729683490162401</v>
+      </c>
+      <c r="T81">
+        <v>51.502352437981003</v>
+      </c>
+      <c r="U81"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="6">
+        <v>29269</v>
+      </c>
+      <c r="I82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="P82">
+        <v>68.824850299400993</v>
+      </c>
+      <c r="T82">
+        <v>97.567365269460907</v>
+      </c>
+      <c r="U82"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="6">
+        <v>29276</v>
+      </c>
+      <c r="I83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="P83">
+        <v>174.18733960650098</v>
+      </c>
+      <c r="T83">
+        <v>150.81800684345501</v>
+      </c>
+      <c r="U83"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="6">
+        <v>29283</v>
+      </c>
+      <c r="I84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="P84">
+        <v>238.21642429426802</v>
+      </c>
+      <c r="T84">
+        <v>130.44803250641499</v>
+      </c>
+      <c r="U84"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>33</v>
+      </c>
+      <c r="B85" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" s="6">
+        <v>29290</v>
+      </c>
+      <c r="I85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="P85">
+        <v>349.00021385799801</v>
+      </c>
+      <c r="T85">
+        <v>102.79619332762999</v>
+      </c>
+      <c r="U85"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" s="6">
+        <v>29297</v>
+      </c>
+      <c r="I86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="P86">
+        <v>366.30667236954599</v>
+      </c>
+      <c r="T86">
+        <v>109.42044482463599</v>
+      </c>
+      <c r="U86"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>35</v>
+      </c>
+      <c r="C87" s="6">
+        <v>29301</v>
+      </c>
+      <c r="I87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="P87">
+        <v>392.86783575705704</v>
+      </c>
+      <c r="T87">
+        <v>98.224978614199898</v>
+      </c>
+      <c r="U87"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I88" s="6"/>
+      <c r="K88" s="6"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I89" s="6"/>
+      <c r="K89" s="6"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I90" s="6"/>
+      <c r="K90" s="6"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I91" s="6"/>
+      <c r="K91" s="6"/>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I92" s="6"/>
+      <c r="K92" s="6"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I93" s="6"/>
+      <c r="K93" s="6"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I94" s="6"/>
+      <c r="K94" s="6"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I95" s="6"/>
+      <c r="K95" s="6"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I96" s="6"/>
+      <c r="K96" s="6"/>
+    </row>
+    <row r="97" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I97" s="6"/>
+      <c r="K97" s="6"/>
+    </row>
+    <row r="98" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I98" s="6"/>
+      <c r="K98" s="6"/>
+    </row>
+    <row r="99" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I99" s="6"/>
+      <c r="K99" s="6"/>
+    </row>
+    <row r="100" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I100" s="6"/>
+      <c r="K100" s="6"/>
+    </row>
+    <row r="101" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I101" s="6"/>
+      <c r="K101" s="6"/>
+    </row>
+    <row r="102" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I102" s="6"/>
+      <c r="K102" s="6"/>
+    </row>
+    <row r="103" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I103" s="6"/>
+      <c r="K103" s="6"/>
+    </row>
+    <row r="104" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I104" s="6"/>
+      <c r="K104" s="6"/>
+    </row>
+    <row r="105" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I105" s="6"/>
+      <c r="K105" s="6"/>
+    </row>
+    <row r="106" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I106" s="6"/>
+      <c r="K106" s="6"/>
+    </row>
+    <row r="107" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I107" s="6"/>
+      <c r="K107" s="6"/>
+    </row>
+    <row r="108" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I108" s="6"/>
+      <c r="K108" s="6"/>
+    </row>
+    <row r="109" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I109" s="6"/>
+      <c r="K109" s="6"/>
+    </row>
+    <row r="110" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I110" s="6"/>
+      <c r="K110" s="6"/>
+    </row>
+    <row r="111" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I111" s="6"/>
+      <c r="K111" s="6"/>
+    </row>
+    <row r="112" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I112" s="6"/>
+      <c r="K112" s="6"/>
+    </row>
+    <row r="113" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I113" s="6"/>
+      <c r="K113" s="6"/>
+    </row>
+    <row r="114" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I114" s="6"/>
+      <c r="K114" s="6"/>
+    </row>
+    <row r="115" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I115" s="6"/>
+      <c r="K115" s="6"/>
+    </row>
+    <row r="116" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I116" s="6"/>
+      <c r="K116" s="6"/>
+    </row>
+    <row r="117" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K117" s="6"/>
+    </row>
+    <row r="118" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K118" s="6"/>
+    </row>
+    <row r="119" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K119" s="6"/>
+    </row>
+    <row r="120" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K120" s="6"/>
+    </row>
+    <row r="121" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K121" s="6"/>
+    </row>
+    <row r="122" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K122" s="6"/>
+    </row>
+    <row r="123" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K123" s="6"/>
+    </row>
+    <row r="124" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K124" s="6"/>
+    </row>
+    <row r="125" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K125" s="6"/>
+    </row>
+    <row r="126" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K126" s="6"/>
+    </row>
+    <row r="127" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K127" s="6"/>
+    </row>
+    <row r="128" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K128" s="6"/>
+    </row>
+    <row r="129" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K129" s="6"/>
+    </row>
+    <row r="130" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K130" s="6"/>
+    </row>
+    <row r="131" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K131" s="6"/>
+    </row>
+    <row r="132" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K132" s="6"/>
+    </row>
+    <row r="133" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K133" s="6"/>
+    </row>
+    <row r="134" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K134" s="6"/>
+    </row>
+    <row r="135" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K135" s="6"/>
+    </row>
+    <row r="136" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K136" s="6"/>
+    </row>
+    <row r="137" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K137" s="6"/>
+    </row>
+    <row r="138" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K138" s="6"/>
+    </row>
+    <row r="139" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K139" s="6"/>
+    </row>
+    <row r="140" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K140" s="6"/>
+    </row>
+    <row r="141" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K141" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W36">
     <sortCondition ref="B2:B36"/>
     <sortCondition ref="C2:C36"/>
   </sortState>

</xml_diff>

<commit_message>
To be pushed-final versions
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/MuchowObserved.xlsx
+++ b/Prototypes/Mungbean/MuchowObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C0D99D-0209-443E-B897-BFEE924365C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF56507-EBC3-498A-BBD2-C1B1CFF4F143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
+    <workbookView xWindow="28680" yWindow="5505" windowWidth="29040" windowHeight="15840" xr2:uid="{0511E703-6483-4FE1-8278-F08B744B2F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="40">
   <si>
     <t>Location</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Mungbean.Grain.Wt</t>
+  </si>
+  <si>
+    <t>Yield</t>
   </si>
 </sst>
 </file>
@@ -553,11 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE48974-63BC-46EF-A3A1-52070277FA63}">
-  <dimension ref="A1:Z141"/>
+  <dimension ref="A1:AA141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,19 +568,19 @@
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="18" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" customWidth="1"/>
-    <col min="21" max="24" width="14.5703125" style="10" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" style="10" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" style="10" customWidth="1"/>
+    <col min="5" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="19" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="25" width="14.5703125" style="10" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="10" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,61 +606,64 @@
         <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -673,11 +679,11 @@
       <c r="F2">
         <v>2.0699999999999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4.53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -687,14 +693,14 @@
       <c r="C3" s="6">
         <v>32918</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>7.18</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -711,7 +717,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -727,11 +733,11 @@
       <c r="F5">
         <v>1.81</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>11.32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -747,42 +753,42 @@
       <c r="H6">
         <v>508</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>13.8</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.05</v>
       </c>
-      <c r="K6">
-        <f>J6/P6</f>
+      <c r="L6">
+        <f>K6/Q6</f>
         <v>4.7169811320754724E-3</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>10.6</v>
       </c>
-      <c r="T6" s="6"/>
-      <c r="U6" s="10">
+      <c r="U6" s="6"/>
+      <c r="V6" s="10">
         <v>264.16000000000003</v>
       </c>
-      <c r="V6" s="10">
+      <c r="W6" s="10">
         <v>243.83999999999997</v>
       </c>
-      <c r="W6" s="10">
+      <c r="X6" s="10">
         <v>10.488000000000001</v>
       </c>
-      <c r="X6" s="10">
+      <c r="Y6" s="10">
         <v>3.3119999999999994</v>
-      </c>
-      <c r="Y6" s="10">
-        <f>W6/U6</f>
-        <v>3.9703210175651121E-2</v>
       </c>
       <c r="Z6" s="10">
         <f>X6/V6</f>
+        <v>3.9703210175651121E-2</v>
+      </c>
+      <c r="AA6" s="10">
+        <f>Y6/W6</f>
         <v>1.3582677165354329E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -798,9 +804,9 @@
       <c r="F7">
         <v>1.81</v>
       </c>
-      <c r="T7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -810,15 +816,15 @@
       <c r="C8" s="6">
         <v>32939</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>5.0199999999999995E-2</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>85.05</v>
       </c>
-      <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -834,12 +840,12 @@
       <c r="F9">
         <v>7.71</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>16.37</v>
       </c>
-      <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -849,18 +855,18 @@
       <c r="C10" s="6">
         <v>32946</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>16.54</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>4.6500000000000007E-2</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>209.13</v>
       </c>
-      <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -876,9 +882,9 @@
       <c r="F11">
         <v>1.31</v>
       </c>
-      <c r="T11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -904,61 +910,65 @@
         <v>827</v>
       </c>
       <c r="I12">
+        <f>P12*10</f>
+        <v>2560</v>
+      </c>
+      <c r="J12">
         <v>18.12</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>12.350000000000001</v>
       </c>
-      <c r="K12">
-        <f>J12/P12</f>
+      <c r="L12">
+        <f>K12/Q12</f>
         <v>3.3324338909875878E-2</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>11.6</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.61440000000000006</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>256</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>370.6</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>50</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>80</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="10">
+      <c r="U12" s="6"/>
+      <c r="V12" s="10">
         <v>169.76000000000002</v>
       </c>
-      <c r="V12" s="10">
-        <f>V6+53.5</f>
+      <c r="W12" s="10">
+        <f>W6+53.5</f>
         <v>297.33999999999997</v>
       </c>
-      <c r="W12" s="10">
+      <c r="X12" s="10">
         <v>3.6180000000000012</v>
       </c>
-      <c r="X12" s="10">
-        <f>X6+1.08</f>
+      <c r="Y12" s="10">
+        <f>Y6+1.08</f>
         <v>4.3919999999999995</v>
-      </c>
-      <c r="Y12" s="10">
-        <f>W12/U12</f>
-        <v>2.1312441093308203E-2</v>
       </c>
       <c r="Z12" s="10">
         <f>X12/V12</f>
+        <v>2.1312441093308203E-2</v>
+      </c>
+      <c r="AA12" s="10">
+        <f>Y12/W12</f>
         <v>1.4770969260778906E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -974,15 +984,15 @@
       <c r="H13">
         <v>226</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>5.53</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>5.34</v>
       </c>
-      <c r="T13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1002,29 +1012,33 @@
         <v>552</v>
       </c>
       <c r="I14">
+        <f>P14*10</f>
+        <v>1550</v>
+      </c>
+      <c r="J14">
         <v>11.5</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>6.54</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>0.32640000000000002</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>155</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>228.34</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>42</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>67</v>
       </c>
-      <c r="T14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1040,15 +1054,15 @@
       <c r="H15">
         <v>273</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5.8</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>12.1</v>
       </c>
-      <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1068,29 +1082,33 @@
         <v>355.7</v>
       </c>
       <c r="I16">
+        <f>P16*10</f>
+        <v>608</v>
+      </c>
+      <c r="J16">
         <v>8.24</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>2.78</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>0.54720000000000002</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>60.8</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>86.399999999999991</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>42</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>63</v>
       </c>
-      <c r="T16" s="6"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U16" s="6"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1100,12 +1118,12 @@
       <c r="C17" s="6">
         <v>32558</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T17" s="6"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U17" s="6"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1115,12 +1133,12 @@
       <c r="C18" s="6">
         <v>32564</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.78</v>
       </c>
-      <c r="T18" s="6"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U18" s="6"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1131,12 +1149,12 @@
         <v>32570</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="I19">
+      <c r="J19">
         <v>3.88</v>
       </c>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U19" s="6"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1152,42 +1170,42 @@
       <c r="H20">
         <v>253</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>7.29</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.22</v>
       </c>
-      <c r="K20">
-        <f>J20/P20</f>
+      <c r="L20">
+        <f>K20/Q20</f>
         <v>4.5081967213114756E-2</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>4.88</v>
       </c>
-      <c r="T20" s="6"/>
-      <c r="U20" s="10">
+      <c r="U20" s="6"/>
+      <c r="V20" s="10">
         <v>134.09</v>
       </c>
-      <c r="V20" s="10">
+      <c r="W20" s="10">
         <v>118.91</v>
       </c>
-      <c r="W20" s="10">
+      <c r="X20" s="10">
         <v>5.9049000000000005</v>
       </c>
-      <c r="X20" s="10">
+      <c r="Y20" s="10">
         <v>1.3850999999999996</v>
-      </c>
-      <c r="Y20" s="10">
-        <f>W20/U20</f>
-        <v>4.4036840927735105E-2</v>
       </c>
       <c r="Z20" s="10">
         <f>X20/V20</f>
+        <v>4.4036840927735105E-2</v>
+      </c>
+      <c r="AA20" s="10">
+        <f>Y20/W20</f>
         <v>1.1648305441089897E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1197,12 +1215,12 @@
       <c r="C21" s="6">
         <v>32585</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>0.05</v>
       </c>
-      <c r="T21" s="6"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U21" s="6"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1212,15 +1230,15 @@
       <c r="C22" s="6">
         <v>32585</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>10.16</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>68.947999999999993</v>
       </c>
-      <c r="T22" s="6"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U22" s="6"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1230,12 +1248,12 @@
       <c r="C23" s="6">
         <v>32592</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>4.5499999999999999E-2</v>
       </c>
-      <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U23" s="6"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1245,15 +1263,15 @@
       <c r="C24" s="6">
         <v>32593</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>10.76</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>165.87700000000001</v>
       </c>
-      <c r="T24" s="6"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U24" s="6"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1273,59 +1291,63 @@
         <v>525</v>
       </c>
       <c r="I25">
+        <f>P25*10</f>
+        <v>1300</v>
+      </c>
+      <c r="J25">
         <v>12.58</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>6.7299999999999995</v>
       </c>
-      <c r="K25">
-        <f>J25/P25</f>
+      <c r="L25">
+        <f>K25/Q25</f>
         <v>3.5074004586199706E-2</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>6.23</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>4.7400000000000005E-2</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.48</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>130</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>191.88</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <v>42</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <v>65</v>
       </c>
-      <c r="T25" s="6"/>
-      <c r="U25" s="10">
+      <c r="U25" s="6"/>
+      <c r="V25" s="10">
         <v>141.55000000000001</v>
       </c>
-      <c r="V25" s="10">
+      <c r="W25" s="10">
         <v>196.20999999999998</v>
       </c>
-      <c r="W25" s="10">
+      <c r="X25" s="10">
         <v>4.3749000000000002</v>
       </c>
-      <c r="X25" s="10">
+      <c r="Y25" s="10">
         <v>1.6850999999999996</v>
-      </c>
-      <c r="Y25" s="10">
-        <f>W25/U25</f>
-        <v>3.090709996467679E-2</v>
       </c>
       <c r="Z25" s="10">
         <f>X25/V25</f>
+        <v>3.090709996467679E-2</v>
+      </c>
+      <c r="AA25" s="10">
+        <f>Y25/W25</f>
         <v>8.5882472860710456E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1335,12 +1357,12 @@
       <c r="C26" s="6">
         <v>32557</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>0.78</v>
       </c>
-      <c r="T26" s="6"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U26" s="6"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1350,12 +1372,12 @@
       <c r="C27" s="6">
         <v>32563</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>2.41</v>
       </c>
-      <c r="T27" s="6"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U27" s="6"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1365,12 +1387,12 @@
       <c r="C28" s="6">
         <v>32569</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>4.04</v>
       </c>
-      <c r="T28" s="6"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U28" s="6"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1380,12 +1402,12 @@
       <c r="C29" s="6">
         <v>32577</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>4.33</v>
       </c>
-      <c r="T29" s="6"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U29" s="6"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1401,42 +1423,42 @@
       <c r="H30">
         <v>180</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>4.1100000000000003</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>0.15</v>
       </c>
-      <c r="K30">
-        <f>J30/P30</f>
+      <c r="L30">
+        <f>K30/Q30</f>
         <v>3.5046728971962614E-2</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>4.28</v>
       </c>
-      <c r="T30" s="6"/>
-      <c r="U30" s="10">
+      <c r="U30" s="6"/>
+      <c r="V30" s="10">
         <v>84.6</v>
       </c>
-      <c r="V30" s="10">
+      <c r="W30" s="10">
         <v>95.4</v>
       </c>
-      <c r="W30" s="10">
+      <c r="X30" s="10">
         <v>3.0825000000000005</v>
       </c>
-      <c r="X30" s="10">
+      <c r="Y30" s="10">
         <v>1.0274999999999999</v>
-      </c>
-      <c r="Y30" s="10">
-        <f>W30/U30</f>
-        <v>3.6436170212765968E-2</v>
       </c>
       <c r="Z30" s="10">
         <f>X30/V30</f>
+        <v>3.6436170212765968E-2</v>
+      </c>
+      <c r="AA30" s="10">
+        <f>Y30/W30</f>
         <v>1.0770440251572325E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1446,12 +1468,12 @@
       <c r="C31" s="6">
         <v>32584</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>4.91</v>
       </c>
-      <c r="T31" s="6"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U31" s="6"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1461,15 +1483,15 @@
       <c r="C32" s="6">
         <v>32585</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>60.91</v>
       </c>
-      <c r="T32" s="6"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U32" s="6"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1479,15 +1501,15 @@
       <c r="C33" s="6">
         <v>32592</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>6.69</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>4.2800000000000005E-2</v>
       </c>
-      <c r="T33" s="6"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U33" s="6"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1497,12 +1519,12 @@
       <c r="C34" s="6">
         <v>32595</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="T34" s="6"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U34" s="6"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1522,56 +1544,60 @@
         <v>349</v>
       </c>
       <c r="I35">
+        <f>P35*10</f>
+        <v>840</v>
+      </c>
+      <c r="J35">
         <v>8.34</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>4.17</v>
       </c>
-      <c r="K35">
-        <f>J35/P35</f>
+      <c r="L35">
+        <f>K35/Q35</f>
         <v>3.3285440613026816E-2</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>3.83</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>0.44160000000000005</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>84</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>125.28</v>
       </c>
-      <c r="R35">
+      <c r="S35">
         <v>42</v>
       </c>
-      <c r="S35">
+      <c r="T35">
         <v>60</v>
       </c>
-      <c r="T35" s="6"/>
-      <c r="U35" s="10">
+      <c r="U35" s="6"/>
+      <c r="V35" s="10">
         <v>91.47</v>
       </c>
-      <c r="V35" s="10">
+      <c r="W35" s="10">
         <v>137.4</v>
       </c>
-      <c r="W35" s="10">
+      <c r="X35" s="10">
         <v>3.0425000000000004</v>
       </c>
-      <c r="X35" s="10">
+      <c r="Y35" s="10">
         <v>1.2074999999999998</v>
-      </c>
-      <c r="Y35" s="10">
-        <f>W35/U35</f>
-        <v>3.3262271783098291E-2</v>
       </c>
       <c r="Z35" s="10">
         <f>X35/V35</f>
+        <v>3.3262271783098291E-2</v>
+      </c>
+      <c r="AA35" s="10">
+        <f>Y35/W35</f>
         <v>8.7882096069868982E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1582,12 +1608,12 @@
         <v>32601</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="I36">
+      <c r="J36">
         <v>12.56</v>
       </c>
-      <c r="T36" s="6"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U36" s="6"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1597,12 +1623,12 @@
       <c r="C37" s="6">
         <v>29262</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="T37">
+      <c r="J37" s="6"/>
+      <c r="U37">
         <v>66.064981949458399</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1612,12 +1638,12 @@
       <c r="C38" s="6">
         <v>29270</v>
       </c>
-      <c r="I38" s="6"/>
-      <c r="T38">
+      <c r="J38" s="6"/>
+      <c r="U38">
         <v>91.046931407942196</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1627,12 +1653,12 @@
       <c r="C39" s="6">
         <v>29279</v>
       </c>
-      <c r="I39" s="6"/>
-      <c r="T39">
+      <c r="J39" s="6"/>
+      <c r="U39">
         <v>81.083032490974702</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1642,12 +1668,12 @@
       <c r="C40" s="6">
         <v>29290</v>
       </c>
-      <c r="I40" s="6"/>
-      <c r="T40">
+      <c r="J40" s="6"/>
+      <c r="U40">
         <v>77.617328519855604</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1657,12 +1683,12 @@
       <c r="C41" s="6">
         <v>29299</v>
       </c>
-      <c r="I41" s="6"/>
-      <c r="T41">
+      <c r="J41" s="6"/>
+      <c r="U41">
         <v>70.974729241877199</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1672,12 +1698,12 @@
       <c r="C42" s="6">
         <v>29262</v>
       </c>
-      <c r="I42" s="6"/>
-      <c r="T42">
+      <c r="J42" s="6"/>
+      <c r="U42">
         <v>84.038004750593899</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -1687,12 +1713,12 @@
       <c r="C43" s="6">
         <v>29270</v>
       </c>
-      <c r="I43" s="6"/>
-      <c r="T43">
+      <c r="J43" s="6"/>
+      <c r="U43">
         <v>96.152019002375397</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1702,12 +1728,12 @@
       <c r="C44" s="6">
         <v>29279</v>
       </c>
-      <c r="I44" s="6"/>
-      <c r="T44">
+      <c r="J44" s="6"/>
+      <c r="U44">
         <v>88.171021377672304</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1717,12 +1743,12 @@
       <c r="C45" s="6">
         <v>29290</v>
       </c>
-      <c r="I45" s="6"/>
-      <c r="T45">
+      <c r="J45" s="6"/>
+      <c r="U45">
         <v>79.762470308788707</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1732,12 +1758,12 @@
       <c r="C46" s="6">
         <v>29299</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="T46">
+      <c r="J46" s="6"/>
+      <c r="U46">
         <v>80.190023752969196</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -1747,12 +1773,12 @@
       <c r="C47" s="6">
         <v>29262</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="T47">
+      <c r="J47" s="6"/>
+      <c r="U47">
         <v>95.107913669064899</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -1762,12 +1788,12 @@
       <c r="C48" s="6">
         <v>29270</v>
       </c>
-      <c r="I48" s="6"/>
-      <c r="T48">
+      <c r="J48" s="6"/>
+      <c r="U48">
         <v>98.561151079136806</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -1777,12 +1803,12 @@
       <c r="C49" s="6">
         <v>29279</v>
       </c>
-      <c r="I49" s="6"/>
-      <c r="T49">
+      <c r="J49" s="6"/>
+      <c r="U49">
         <v>97.410071942446095</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -1792,12 +1818,12 @@
       <c r="C50" s="6">
         <v>29290</v>
       </c>
-      <c r="I50" s="6"/>
-      <c r="T50">
+      <c r="J50" s="6"/>
+      <c r="U50">
         <v>91.654676258992893</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1807,12 +1833,12 @@
       <c r="C51" s="6">
         <v>29299</v>
       </c>
-      <c r="I51" s="6"/>
-      <c r="T51">
+      <c r="J51" s="6"/>
+      <c r="U51">
         <v>91.366906474820297</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -1825,11 +1851,11 @@
       <c r="H52">
         <v>0.32111198190552498</v>
       </c>
-      <c r="I52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="T52" s="6"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="U52" s="6"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1842,11 +1868,11 @@
       <c r="H53">
         <v>1.09776133645736</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="T53" s="6"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="U53" s="6"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1859,11 +1885,11 @@
       <c r="H54">
         <v>1.7268245737280801</v>
       </c>
-      <c r="I54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="T54" s="6"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="U54" s="6"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -1876,11 +1902,11 @@
       <c r="H55">
         <v>2.7213304475296698</v>
       </c>
-      <c r="I55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="T55" s="6"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="U55" s="6"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -1893,11 +1919,11 @@
       <c r="H56">
         <v>4.1666551613518799</v>
       </c>
-      <c r="I56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="T56" s="6"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="U56" s="6"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -1910,11 +1936,11 @@
       <c r="H57">
         <v>4.9589382083382398</v>
       </c>
-      <c r="I57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="T57" s="6"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="U57" s="6"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -1927,11 +1953,11 @@
       <c r="H58">
         <v>4.9658210937087599</v>
       </c>
-      <c r="I58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="T58" s="6"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="U58" s="6"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -1944,17 +1970,17 @@
       <c r="H59">
         <v>6.2712953224804302</v>
       </c>
-      <c r="I59" s="6"/>
-      <c r="L59" s="6"/>
-      <c r="P59">
+      <c r="J59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="Q59">
         <v>19.285714285714199</v>
       </c>
-      <c r="R59">
+      <c r="S59">
         <v>5.4533789563713199E-3</v>
       </c>
-      <c r="T59" s="6"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U59" s="6"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -1967,17 +1993,17 @@
       <c r="H60">
         <v>6.0141515371777299</v>
       </c>
-      <c r="I60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="P60">
+      <c r="J60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="Q60">
         <v>26.071428571428601</v>
       </c>
-      <c r="R60">
+      <c r="S60">
         <v>0.125106928999143</v>
       </c>
-      <c r="T60" s="6"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U60" s="6"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -1990,17 +2016,17 @@
       <c r="H61">
         <v>0.16554659043380501</v>
       </c>
-      <c r="I61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="P61">
+      <c r="J61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="Q61">
         <v>31.964285714285701</v>
       </c>
-      <c r="R61">
+      <c r="S61">
         <v>0.51502352437981003</v>
       </c>
-      <c r="T61" s="6"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U61" s="6"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2013,17 +2039,17 @@
       <c r="H62">
         <v>0.48347904476108899</v>
       </c>
-      <c r="I62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="P62">
+      <c r="J62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="Q62">
         <v>39.107142857142797</v>
       </c>
-      <c r="R62">
+      <c r="S62">
         <v>0.97567365269460904</v>
       </c>
-      <c r="T62" s="6"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U62" s="6"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2036,17 +2062,17 @@
       <c r="H63">
         <v>1.1902640672776601</v>
       </c>
-      <c r="I63" s="6"/>
-      <c r="L63" s="6"/>
-      <c r="P63">
+      <c r="J63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="Q63">
         <v>46.25</v>
       </c>
-      <c r="R63">
+      <c r="S63">
         <v>1.5081800684345501</v>
       </c>
-      <c r="T63" s="6"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U63" s="6"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -2059,17 +2085,17 @@
       <c r="H64">
         <v>2.27820663274629</v>
       </c>
-      <c r="I64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="P64">
+      <c r="J64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="Q64">
         <v>53.035714285714299</v>
       </c>
-      <c r="R64">
+      <c r="S64">
         <v>1.3044803250641499</v>
       </c>
-      <c r="T64" s="6"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U64" s="6"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -2082,17 +2108,17 @@
       <c r="H65">
         <v>3.7157348038479201</v>
       </c>
-      <c r="I65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="P65">
+      <c r="J65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="Q65">
         <v>60.892857142857103</v>
       </c>
-      <c r="R65">
+      <c r="S65">
         <v>1.0279619332762999</v>
       </c>
-      <c r="T65" s="6"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U65" s="6"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -2105,17 +2131,17 @@
       <c r="H66">
         <v>4.1968667643941604</v>
       </c>
-      <c r="I66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="P66">
+      <c r="J66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="Q66">
         <v>67.142857142857196</v>
       </c>
-      <c r="R66">
+      <c r="S66">
         <v>1.09420444824636</v>
       </c>
-      <c r="T66" s="6"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U66" s="6"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -2128,17 +2154,17 @@
       <c r="H67">
         <v>5.0824240750742096</v>
       </c>
-      <c r="I67" s="6"/>
-      <c r="L67" s="6"/>
-      <c r="P67">
+      <c r="J67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="Q67">
         <v>71.785714285714306</v>
       </c>
-      <c r="R67">
+      <c r="S67">
         <v>0.98224978614199898</v>
       </c>
-      <c r="T67" s="6"/>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U67" s="6"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -2151,17 +2177,17 @@
       <c r="H68">
         <v>5.29152978725996</v>
       </c>
-      <c r="I68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="P68">
+      <c r="J68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="Q68">
         <v>19.285714285714199</v>
       </c>
-      <c r="R68">
+      <c r="S68">
         <v>0</v>
       </c>
-      <c r="T68" s="6"/>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U68" s="6"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2174,16 +2200,16 @@
       <c r="H69">
         <v>5.4775910307273099</v>
       </c>
-      <c r="I69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="P69">
+      <c r="J69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="Q69">
         <v>26.071428571428601</v>
       </c>
-      <c r="R69">
+      <c r="S69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -2196,16 +2222,16 @@
       <c r="H70">
         <v>8.7743591201277796E-2</v>
       </c>
-      <c r="I70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="P70">
+      <c r="J70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="Q70">
         <v>32.5</v>
       </c>
-      <c r="R70">
+      <c r="S70">
         <v>0.137296834901624</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2218,16 +2244,16 @@
       <c r="H71">
         <v>0.226863150371757</v>
       </c>
-      <c r="I71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="P71">
+      <c r="J71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="Q71">
         <v>39.107142857142797</v>
       </c>
-      <c r="R71">
+      <c r="S71">
         <v>0.68824850299400997</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2240,16 +2266,16 @@
       <c r="H72">
         <v>0.73926249578702496</v>
       </c>
-      <c r="I72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="P72">
+      <c r="J72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="Q72">
         <v>46.071428571428598</v>
       </c>
-      <c r="R72">
+      <c r="S72">
         <v>1.7418733960650099</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -2262,16 +2288,16 @@
       <c r="H73">
         <v>1.3528341650999101</v>
       </c>
-      <c r="I73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="P73">
+      <c r="J73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="Q73">
         <v>53.214285714285701</v>
       </c>
-      <c r="R73">
+      <c r="S73">
         <v>2.3821642429426801</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -2284,16 +2310,16 @@
       <c r="H74">
         <v>2.6347969447298198</v>
       </c>
-      <c r="I74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="P74">
+      <c r="J74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="Q74">
         <v>59.821428571428498</v>
       </c>
-      <c r="R74">
+      <c r="S74">
         <v>3.49000213857998</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -2306,16 +2332,16 @@
       <c r="H75">
         <v>3.7147399325111699</v>
       </c>
-      <c r="I75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="P75">
+      <c r="J75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="Q75">
         <v>67.142857142857196</v>
       </c>
-      <c r="R75">
+      <c r="S75">
         <v>3.6630667236954602</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -2328,16 +2354,16 @@
       <c r="H76">
         <v>4.1103738685876401</v>
       </c>
-      <c r="I76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="P76">
+      <c r="J76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="Q76">
         <v>71.428571428571402</v>
       </c>
-      <c r="R76">
+      <c r="S76">
         <v>3.9286783575705702</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -2350,10 +2376,10 @@
       <c r="H77">
         <v>5.1981743095795903</v>
       </c>
-      <c r="I77" s="6"/>
-      <c r="L77" s="6"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J77" s="6"/>
+      <c r="M77" s="6"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -2366,10 +2392,10 @@
       <c r="H78">
         <v>5.3687033780957698</v>
       </c>
-      <c r="I78" s="6"/>
-      <c r="L78" s="6"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J78" s="6"/>
+      <c r="M78" s="6"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -2379,17 +2405,17 @@
       <c r="C79" s="6">
         <v>29249</v>
       </c>
-      <c r="I79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="Q79">
+      <c r="J79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="R79">
         <v>0</v>
       </c>
-      <c r="U79">
+      <c r="V79">
         <v>0.54533789563713198</v>
       </c>
-      <c r="V79"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W79"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -2399,17 +2425,17 @@
       <c r="C80" s="6">
         <v>29256</v>
       </c>
-      <c r="I80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="Q80">
+      <c r="J80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="R80">
         <v>0</v>
       </c>
-      <c r="U80">
+      <c r="V80">
         <v>12.5106928999143</v>
       </c>
-      <c r="V80"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W80"/>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -2419,17 +2445,17 @@
       <c r="C81" s="6">
         <v>29262</v>
       </c>
-      <c r="I81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="Q81">
+      <c r="J81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="R81">
         <v>13.729683490162401</v>
       </c>
-      <c r="U81">
+      <c r="V81">
         <v>51.502352437981003</v>
       </c>
-      <c r="V81"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W81"/>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -2439,17 +2465,17 @@
       <c r="C82" s="6">
         <v>29269</v>
       </c>
-      <c r="I82" s="6"/>
-      <c r="L82" s="6"/>
-      <c r="Q82">
+      <c r="J82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="R82">
         <v>68.824850299400993</v>
       </c>
-      <c r="U82">
+      <c r="V82">
         <v>97.567365269460907</v>
       </c>
-      <c r="V82"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W82"/>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2459,17 +2485,17 @@
       <c r="C83" s="6">
         <v>29276</v>
       </c>
-      <c r="I83" s="6"/>
-      <c r="L83" s="6"/>
-      <c r="Q83">
+      <c r="J83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="R83">
         <v>174.18733960650098</v>
       </c>
-      <c r="U83">
+      <c r="V83">
         <v>150.81800684345501</v>
       </c>
-      <c r="V83"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W83"/>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -2479,17 +2505,17 @@
       <c r="C84" s="6">
         <v>29283</v>
       </c>
-      <c r="I84" s="6"/>
-      <c r="L84" s="6"/>
-      <c r="Q84">
+      <c r="J84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="R84">
         <v>238.21642429426802</v>
       </c>
-      <c r="U84">
+      <c r="V84">
         <v>130.44803250641499</v>
       </c>
-      <c r="V84"/>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W84"/>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -2499,17 +2525,17 @@
       <c r="C85" s="6">
         <v>29290</v>
       </c>
-      <c r="I85" s="6"/>
-      <c r="L85" s="6"/>
-      <c r="Q85">
+      <c r="J85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="R85">
         <v>349.00021385799801</v>
       </c>
-      <c r="U85">
+      <c r="V85">
         <v>102.79619332762999</v>
       </c>
-      <c r="V85"/>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W85"/>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -2519,17 +2545,17 @@
       <c r="C86" s="6">
         <v>29297</v>
       </c>
-      <c r="I86" s="6"/>
-      <c r="L86" s="6"/>
-      <c r="Q86">
+      <c r="J86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="R86">
         <v>366.30667236954599</v>
       </c>
-      <c r="U86">
+      <c r="V86">
         <v>109.42044482463599</v>
       </c>
-      <c r="V86"/>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W86"/>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -2539,209 +2565,209 @@
       <c r="C87" s="6">
         <v>29301</v>
       </c>
-      <c r="I87" s="6"/>
-      <c r="L87" s="6"/>
-      <c r="Q87">
+      <c r="J87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="R87">
         <v>392.86783575705704</v>
       </c>
-      <c r="U87">
+      <c r="V87">
         <v>98.224978614199898</v>
       </c>
-      <c r="V87"/>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I88" s="6"/>
-      <c r="L88" s="6"/>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I89" s="6"/>
-      <c r="L89" s="6"/>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I90" s="6"/>
-      <c r="L90" s="6"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I91" s="6"/>
-      <c r="L91" s="6"/>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I92" s="6"/>
-      <c r="L92" s="6"/>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I93" s="6"/>
-      <c r="L93" s="6"/>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I94" s="6"/>
-      <c r="L94" s="6"/>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I95" s="6"/>
-      <c r="L95" s="6"/>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I96" s="6"/>
-      <c r="L96" s="6"/>
-    </row>
-    <row r="97" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I97" s="6"/>
-      <c r="L97" s="6"/>
-    </row>
-    <row r="98" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I98" s="6"/>
-      <c r="L98" s="6"/>
-    </row>
-    <row r="99" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I99" s="6"/>
-      <c r="L99" s="6"/>
-    </row>
-    <row r="100" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I100" s="6"/>
-      <c r="L100" s="6"/>
-    </row>
-    <row r="101" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I101" s="6"/>
-      <c r="L101" s="6"/>
-    </row>
-    <row r="102" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I102" s="6"/>
-      <c r="L102" s="6"/>
-    </row>
-    <row r="103" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I103" s="6"/>
-      <c r="L103" s="6"/>
-    </row>
-    <row r="104" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I104" s="6"/>
-      <c r="L104" s="6"/>
-    </row>
-    <row r="105" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I105" s="6"/>
-      <c r="L105" s="6"/>
-    </row>
-    <row r="106" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I106" s="6"/>
-      <c r="L106" s="6"/>
-    </row>
-    <row r="107" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I107" s="6"/>
-      <c r="L107" s="6"/>
-    </row>
-    <row r="108" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I108" s="6"/>
-      <c r="L108" s="6"/>
-    </row>
-    <row r="109" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I109" s="6"/>
-      <c r="L109" s="6"/>
-    </row>
-    <row r="110" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I110" s="6"/>
-      <c r="L110" s="6"/>
-    </row>
-    <row r="111" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I111" s="6"/>
-      <c r="L111" s="6"/>
-    </row>
-    <row r="112" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I112" s="6"/>
-      <c r="L112" s="6"/>
-    </row>
-    <row r="113" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I113" s="6"/>
-      <c r="L113" s="6"/>
-    </row>
-    <row r="114" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I114" s="6"/>
-      <c r="L114" s="6"/>
-    </row>
-    <row r="115" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I115" s="6"/>
-      <c r="L115" s="6"/>
-    </row>
-    <row r="116" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I116" s="6"/>
-      <c r="L116" s="6"/>
-    </row>
-    <row r="117" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L117" s="6"/>
-    </row>
-    <row r="118" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L118" s="6"/>
-    </row>
-    <row r="119" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L119" s="6"/>
-    </row>
-    <row r="120" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L120" s="6"/>
-    </row>
-    <row r="121" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L121" s="6"/>
-    </row>
-    <row r="122" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L122" s="6"/>
-    </row>
-    <row r="123" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L123" s="6"/>
-    </row>
-    <row r="124" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L124" s="6"/>
-    </row>
-    <row r="125" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L125" s="6"/>
-    </row>
-    <row r="126" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L126" s="6"/>
-    </row>
-    <row r="127" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L127" s="6"/>
-    </row>
-    <row r="128" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L128" s="6"/>
-    </row>
-    <row r="129" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L129" s="6"/>
-    </row>
-    <row r="130" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L130" s="6"/>
-    </row>
-    <row r="131" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L131" s="6"/>
-    </row>
-    <row r="132" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L132" s="6"/>
-    </row>
-    <row r="133" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L133" s="6"/>
-    </row>
-    <row r="134" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L134" s="6"/>
-    </row>
-    <row r="135" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L135" s="6"/>
-    </row>
-    <row r="136" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L136" s="6"/>
-    </row>
-    <row r="137" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L137" s="6"/>
-    </row>
-    <row r="138" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L138" s="6"/>
-    </row>
-    <row r="139" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L139" s="6"/>
-    </row>
-    <row r="140" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L140" s="6"/>
-    </row>
-    <row r="141" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L141" s="6"/>
+      <c r="W87"/>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J88" s="6"/>
+      <c r="M88" s="6"/>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J89" s="6"/>
+      <c r="M89" s="6"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J90" s="6"/>
+      <c r="M90" s="6"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J91" s="6"/>
+      <c r="M91" s="6"/>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J92" s="6"/>
+      <c r="M92" s="6"/>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J93" s="6"/>
+      <c r="M93" s="6"/>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J94" s="6"/>
+      <c r="M94" s="6"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J95" s="6"/>
+      <c r="M95" s="6"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J96" s="6"/>
+      <c r="M96" s="6"/>
+    </row>
+    <row r="97" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J97" s="6"/>
+      <c r="M97" s="6"/>
+    </row>
+    <row r="98" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J98" s="6"/>
+      <c r="M98" s="6"/>
+    </row>
+    <row r="99" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J99" s="6"/>
+      <c r="M99" s="6"/>
+    </row>
+    <row r="100" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J100" s="6"/>
+      <c r="M100" s="6"/>
+    </row>
+    <row r="101" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J101" s="6"/>
+      <c r="M101" s="6"/>
+    </row>
+    <row r="102" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J102" s="6"/>
+      <c r="M102" s="6"/>
+    </row>
+    <row r="103" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J103" s="6"/>
+      <c r="M103" s="6"/>
+    </row>
+    <row r="104" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J104" s="6"/>
+      <c r="M104" s="6"/>
+    </row>
+    <row r="105" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J105" s="6"/>
+      <c r="M105" s="6"/>
+    </row>
+    <row r="106" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J106" s="6"/>
+      <c r="M106" s="6"/>
+    </row>
+    <row r="107" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J107" s="6"/>
+      <c r="M107" s="6"/>
+    </row>
+    <row r="108" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J108" s="6"/>
+      <c r="M108" s="6"/>
+    </row>
+    <row r="109" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J109" s="6"/>
+      <c r="M109" s="6"/>
+    </row>
+    <row r="110" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J110" s="6"/>
+      <c r="M110" s="6"/>
+    </row>
+    <row r="111" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J111" s="6"/>
+      <c r="M111" s="6"/>
+    </row>
+    <row r="112" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J112" s="6"/>
+      <c r="M112" s="6"/>
+    </row>
+    <row r="113" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J113" s="6"/>
+      <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J114" s="6"/>
+      <c r="M114" s="6"/>
+    </row>
+    <row r="115" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J115" s="6"/>
+      <c r="M115" s="6"/>
+    </row>
+    <row r="116" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J116" s="6"/>
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M117" s="6"/>
+    </row>
+    <row r="118" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M118" s="6"/>
+    </row>
+    <row r="119" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M119" s="6"/>
+    </row>
+    <row r="120" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M120" s="6"/>
+    </row>
+    <row r="121" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M121" s="6"/>
+    </row>
+    <row r="122" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M122" s="6"/>
+    </row>
+    <row r="123" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M123" s="6"/>
+    </row>
+    <row r="124" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M124" s="6"/>
+    </row>
+    <row r="125" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M125" s="6"/>
+    </row>
+    <row r="126" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M126" s="6"/>
+    </row>
+    <row r="127" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M127" s="6"/>
+    </row>
+    <row r="128" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="M128" s="6"/>
+    </row>
+    <row r="129" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M129" s="6"/>
+    </row>
+    <row r="130" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M130" s="6"/>
+    </row>
+    <row r="131" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M131" s="6"/>
+    </row>
+    <row r="132" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M132" s="6"/>
+    </row>
+    <row r="133" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M133" s="6"/>
+    </row>
+    <row r="134" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M134" s="6"/>
+    </row>
+    <row r="135" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M135" s="6"/>
+    </row>
+    <row r="136" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M136" s="6"/>
+    </row>
+    <row r="137" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M137" s="6"/>
+    </row>
+    <row r="138" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M138" s="6"/>
+    </row>
+    <row r="139" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M139" s="6"/>
+    </row>
+    <row r="140" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M140" s="6"/>
+    </row>
+    <row r="141" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M141" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y36">
     <sortCondition ref="B2:B36"/>
     <sortCondition ref="C2:C36"/>
   </sortState>

</xml_diff>